<commit_message>
terminado metodos basicos de la clase controlarExcel !importante cambio de sqlite a excel en pandas
</commit_message>
<xml_diff>
--- a/core/openYdelTablas/prueba.xlsx
+++ b/core/openYdelTablas/prueba.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,6 +435,13 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bendezu</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
terminando las funcionalidad extras de la clase controladorDeEX
</commit_message>
<xml_diff>
--- a/core/openYdelTablas/prueba.xlsx
+++ b/core/openYdelTablas/prueba.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,21 +424,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>apellidos</t>
+          <t>nombre</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
-          <t>moreno</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>bendezu</t>
+          <t>apellido</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
mejorando la interaccion con variables
</commit_message>
<xml_diff>
--- a/core/openYdelTablas/prueba.xlsx
+++ b/core/openYdelTablas/prueba.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,6 +433,30 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>randu</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>condori</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>randu</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>condori</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>